<commit_message>
Upload for Assignment 04
</commit_message>
<xml_diff>
--- a/docs/GARERI.Asg04.TimeChart.xlsx
+++ b/docs/GARERI.Asg04.TimeChart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcgar\Documents\Coursework2022\Summer\CS372\Assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcgar\source\repos\cs372.gareri\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F216A6B-0F2D-4B74-B134-53C2101AF867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F825A942-D266-488C-945B-FE6A6EA1A4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0231567D-3562-4E41-810A-4666E8665883}"/>
+    <workbookView xWindow="6156" yWindow="1356" windowWidth="17280" windowHeight="8880" xr2:uid="{0231567D-3562-4E41-810A-4666E8665883}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -319,16 +319,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.36993E-2</c:v>
+                  <c:v>1.04888E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32467000000000001</c:v>
+                  <c:v>1.0105999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.8828399999999998</c:v>
+                  <c:v>7.6022999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>116.429</c:v>
+                  <c:v>115.51600000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3762.06</c:v>
@@ -388,16 +388,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.36993E-2</c:v>
+                  <c:v>9.9127E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32467000000000001</c:v>
+                  <c:v>0.97249799999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.8828399999999998</c:v>
+                  <c:v>3.8354300000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>116.429</c:v>
+                  <c:v>111.271</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3762.06</c:v>
@@ -1537,7 +1537,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1564,10 +1564,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>2.36993E-2</v>
+        <v>1.04888E-2</v>
       </c>
       <c r="C2" s="2">
-        <v>2.36993E-2</v>
+        <v>9.9127E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1575,10 +1575,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>0.32467000000000001</v>
+        <v>1.0105999999999999</v>
       </c>
       <c r="C3" s="2">
-        <v>0.32467000000000001</v>
+        <v>0.97249799999999997</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1586,10 +1586,10 @@
         <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>7.8828399999999998</v>
+        <v>7.6022999999999996</v>
       </c>
       <c r="C4" s="2">
-        <v>7.8828399999999998</v>
+        <v>3.8354300000000001</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1597,10 +1597,10 @@
         <v>20</v>
       </c>
       <c r="B5" s="2">
-        <v>116.429</v>
+        <v>115.51600000000001</v>
       </c>
       <c r="C5" s="2">
-        <v>116.429</v>
+        <v>111.271</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>